<commit_message>
chore: add has children
</commit_message>
<xml_diff>
--- a/outputs/output.xlsx
+++ b/outputs/output.xlsx
@@ -155,7 +155,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -311,7 +311,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -479,7 +479,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -567,7 +567,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -819,7 +819,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -1131,7 +1131,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -1939,7 +1939,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -2439,7 +2439,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -2527,7 +2527,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -2573,7 +2573,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -2851,7 +2851,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -3721,7 +3721,7 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -4707,7 +4707,7 @@
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -5061,7 +5061,7 @@
       </c>
       <c r="J123" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -5645,7 +5645,7 @@
       </c>
       <c r="J137" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -5843,7 +5843,7 @@
       </c>
       <c r="J142" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -5935,7 +5935,7 @@
       </c>
       <c r="J144" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -5981,7 +5981,7 @@
       </c>
       <c r="J145" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -6203,7 +6203,7 @@
       </c>
       <c r="J150" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -6439,7 +6439,7 @@
       </c>
       <c r="J156" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -6561,7 +6561,7 @@
       </c>
       <c r="J159" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -6863,7 +6863,7 @@
       </c>
       <c r="J166" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -7377,7 +7377,7 @@
       </c>
       <c r="J179" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -7671,7 +7671,7 @@
       </c>
       <c r="J186" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -7865,7 +7865,7 @@
       </c>
       <c r="J191" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8291,7 +8291,7 @@
       </c>
       <c r="J202" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8657,7 +8657,7 @@
       </c>
       <c r="J211" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8909,7 +8909,7 @@
       </c>
       <c r="J217" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -9807,7 +9807,7 @@
       </c>
       <c r="J240" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -9975,7 +9975,7 @@
       </c>
       <c r="J244" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -10859,7 +10859,7 @@
       </c>
       <c r="J266" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -10947,7 +10947,7 @@
       </c>
       <c r="J268" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -10993,7 +10993,7 @@
       </c>
       <c r="J269" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -11039,7 +11039,7 @@
       </c>
       <c r="J270" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -11309,7 +11309,7 @@
       </c>
       <c r="J277" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -11439,7 +11439,7 @@
       </c>
       <c r="J280" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -11523,7 +11523,7 @@
       </c>
       <c r="J282" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -11763,7 +11763,7 @@
       </c>
       <c r="J288" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -12027,7 +12027,7 @@
       </c>
       <c r="J294" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -12359,7 +12359,7 @@
       </c>
       <c r="J302" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -12447,7 +12447,7 @@
       </c>
       <c r="J304" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -12489,7 +12489,7 @@
       </c>
       <c r="J305" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -13239,7 +13239,7 @@
       </c>
       <c r="J324" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -13513,7 +13513,7 @@
       </c>
       <c r="J331" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -13559,7 +13559,7 @@
       </c>
       <c r="J332" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -13951,7 +13951,7 @@
       </c>
       <c r="J342" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -14141,7 +14141,7 @@
       </c>
       <c r="J347" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -14475,7 +14475,7 @@
       </c>
       <c r="J356" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -14761,7 +14761,7 @@
       </c>
       <c r="J363" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -14807,7 +14807,7 @@
       </c>
       <c r="J364" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -14921,7 +14921,7 @@
       </c>
       <c r="J367" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -15211,7 +15211,7 @@
       </c>
       <c r="J374" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -15593,7 +15593,7 @@
       </c>
       <c r="J383" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -15841,7 +15841,7 @@
       </c>
       <c r="J389" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -16081,7 +16081,7 @@
       </c>
       <c r="J395" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -16477,7 +16477,7 @@
       </c>
       <c r="J405" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -16607,7 +16607,7 @@
       </c>
       <c r="J408" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -16775,7 +16775,7 @@
       </c>
       <c r="J412" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -16985,7 +16985,7 @@
       </c>
       <c r="J417" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -17179,7 +17179,7 @@
       </c>
       <c r="J422" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -17485,7 +17485,7 @@
       </c>
       <c r="J429" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -17855,7 +17855,7 @@
       </c>
       <c r="J438" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -17905,7 +17905,7 @@
       </c>
       <c r="J439" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -18103,7 +18103,7 @@
       </c>
       <c r="J444" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -18149,7 +18149,7 @@
       </c>
       <c r="J445" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -18279,7 +18279,7 @@
       </c>
       <c r="J448" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -18325,7 +18325,7 @@
       </c>
       <c r="J449" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -18577,7 +18577,7 @@
       </c>
       <c r="J455" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -19011,7 +19011,7 @@
       </c>
       <c r="J466" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -19137,7 +19137,7 @@
       </c>
       <c r="J469" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -19221,7 +19221,7 @@
       </c>
       <c r="J471" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -19343,7 +19343,7 @@
       </c>
       <c r="J474" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -19431,7 +19431,7 @@
       </c>
       <c r="J476" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -19477,7 +19477,7 @@
       </c>
       <c r="J477" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -19611,7 +19611,7 @@
       </c>
       <c r="J480" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -19825,7 +19825,7 @@
       </c>
       <c r="J485" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -20035,7 +20035,7 @@
       </c>
       <c r="J490" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -20493,7 +20493,7 @@
       </c>
       <c r="J501" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>

</xml_diff>